<commit_message>
update meme prediect motif
</commit_message>
<xml_diff>
--- a/序列信息.xlsx
+++ b/序列信息.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -502,7 +502,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="G2" sqref="G2:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>